<commit_message>
trimmed PCAs on trim mastersheet
</commit_message>
<xml_diff>
--- a/data/trimmed_Monthly Mastersheet Original Data.xlsx
+++ b/data/trimmed_Monthly Mastersheet Original Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aliceye/Desktop/CryptoMacroecon-Prediction-CSUREMM/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8C245DE2-0896-8A47-A287-49C439A50BAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6FABB27-2733-4946-8C00-1992A57EC4ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2680" yWindow="3260" windowWidth="26040" windowHeight="14740" xr2:uid="{D037DA27-6BB7-AE4D-A438-2863195A8A2D}"/>
+    <workbookView xWindow="1380" yWindow="760" windowWidth="26040" windowHeight="14740" xr2:uid="{D037DA27-6BB7-AE4D-A438-2863195A8A2D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Month</t>
   </si>
@@ -87,6 +87,18 @@
   </si>
   <si>
     <t>GDP</t>
+  </si>
+  <si>
+    <t>PC1_macro</t>
+  </si>
+  <si>
+    <t>PC2_macro</t>
+  </si>
+  <si>
+    <t>PC1_crypto</t>
+  </si>
+  <si>
+    <t>PC2_crypto</t>
   </si>
 </sst>
 </file>
@@ -143,7 +155,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -188,11 +200,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="17" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -206,6 +227,9 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -542,15 +566,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC2EB1B9-0B7B-B649-BF34-64FC2B00F027}">
-  <dimension ref="A1:Q57"/>
+  <dimension ref="A1:U57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="S9" sqref="S9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="V5" sqref="V5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -602,8 +626,20 @@
       <c r="Q1" s="6" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R1" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" s="7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>43983</v>
       </c>
@@ -655,8 +691,20 @@
       <c r="Q2" s="2">
         <v>19942.07</v>
       </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R2">
+        <v>18898.159859685391</v>
+      </c>
+      <c r="S2">
+        <v>-16745.070827052768</v>
+      </c>
+      <c r="T2">
+        <v>4.0346425946562734</v>
+      </c>
+      <c r="U2">
+        <v>0.36336360296791281</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>44013</v>
       </c>
@@ -708,8 +756,20 @@
       <c r="Q3" s="2">
         <v>20373.16</v>
       </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R3">
+        <v>19224.388531274359</v>
+      </c>
+      <c r="S3">
+        <v>-17335.648706597989</v>
+      </c>
+      <c r="T3">
+        <v>5.0116280582367736</v>
+      </c>
+      <c r="U3">
+        <v>0.63774288661647804</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>44044</v>
       </c>
@@ -761,8 +821,20 @@
       <c r="Q4" s="2">
         <v>20531.23</v>
       </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R4">
+        <v>19343.986618652001</v>
+      </c>
+      <c r="S4">
+        <v>-17461.336191074919</v>
+      </c>
+      <c r="T4">
+        <v>3.3049332739107262</v>
+      </c>
+      <c r="U4">
+        <v>1.7287633053973579</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>44075</v>
       </c>
@@ -814,8 +886,20 @@
       <c r="Q5" s="2">
         <v>20745.2</v>
       </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R5">
+        <v>19648.942574136199</v>
+      </c>
+      <c r="S5">
+        <v>-17612.768747837381</v>
+      </c>
+      <c r="T5">
+        <v>3.7855928171679301</v>
+      </c>
+      <c r="U5">
+        <v>0.81737013204221531</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>44105</v>
       </c>
@@ -867,8 +951,20 @@
       <c r="Q6" s="2">
         <v>20868.45</v>
       </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R6">
+        <v>19828.763353704431</v>
+      </c>
+      <c r="S6">
+        <v>-17829.15051402256</v>
+      </c>
+      <c r="T6">
+        <v>3.6013145131629631</v>
+      </c>
+      <c r="U6">
+        <v>0.40465515504101801</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>44136</v>
       </c>
@@ -920,8 +1016,20 @@
       <c r="Q7" s="2">
         <v>20654.25</v>
       </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R7">
+        <v>20123.608833005848</v>
+      </c>
+      <c r="S7">
+        <v>-17599.173451688919</v>
+      </c>
+      <c r="T7">
+        <v>5.2771994093212147</v>
+      </c>
+      <c r="U7">
+        <v>0.2006908060245565</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>44166</v>
       </c>
@@ -973,8 +1081,20 @@
       <c r="Q8" s="2">
         <v>20795.82</v>
       </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R8">
+        <v>20453.988213287561</v>
+      </c>
+      <c r="S8">
+        <v>-17682.5696533995</v>
+      </c>
+      <c r="T8">
+        <v>2.6052837265179258</v>
+      </c>
+      <c r="U8">
+        <v>0.6584713510560225</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>44197</v>
       </c>
@@ -1026,8 +1146,20 @@
       <c r="Q9" s="2">
         <v>21116.94</v>
       </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R9">
+        <v>20645.158867623461</v>
+      </c>
+      <c r="S9">
+        <v>-18031.833849187169</v>
+      </c>
+      <c r="T9">
+        <v>2.4646666404426258</v>
+      </c>
+      <c r="U9">
+        <v>0.73775990613938214</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>44228</v>
       </c>
@@ -1079,8 +1211,20 @@
       <c r="Q10" s="2">
         <v>20812.89</v>
       </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R10">
+        <v>20728.651121855961</v>
+      </c>
+      <c r="S10">
+        <v>-17749.166318029969</v>
+      </c>
+      <c r="T10">
+        <v>1.080131176728832</v>
+      </c>
+      <c r="U10">
+        <v>1.597578269986387</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>44256</v>
       </c>
@@ -1132,8 +1276,20 @@
       <c r="Q11" s="2">
         <v>21249.16</v>
       </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R11">
+        <v>21214.35140101787</v>
+      </c>
+      <c r="S11">
+        <v>-18075.7155097248</v>
+      </c>
+      <c r="T11">
+        <v>1.9872335641764489</v>
+      </c>
+      <c r="U11">
+        <v>1.042133969392381</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>44287</v>
       </c>
@@ -1185,8 +1341,20 @@
       <c r="Q12" s="2">
         <v>21366.84</v>
       </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R12">
+        <v>21664.6513709674</v>
+      </c>
+      <c r="S12">
+        <v>-18217.518670257621</v>
+      </c>
+      <c r="T12">
+        <v>3.20064267155648</v>
+      </c>
+      <c r="U12">
+        <v>0.80294359179841102</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>44317</v>
       </c>
@@ -1238,8 +1406,20 @@
       <c r="Q13" s="2">
         <v>21372.81</v>
       </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R13">
+        <v>21739.742085584909</v>
+      </c>
+      <c r="S13">
+        <v>-18213.087255933151</v>
+      </c>
+      <c r="T13">
+        <v>1.9667768354592701</v>
+      </c>
+      <c r="U13">
+        <v>1.7080709315477951</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>44348</v>
       </c>
@@ -1291,8 +1471,20 @@
       <c r="Q14" s="2">
         <v>21431.14</v>
       </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R14">
+        <v>21883.364234914949</v>
+      </c>
+      <c r="S14">
+        <v>-18246.498216066859</v>
+      </c>
+      <c r="T14">
+        <v>1.131142131985869</v>
+      </c>
+      <c r="U14">
+        <v>0.58548690962253747</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>44378</v>
       </c>
@@ -1344,8 +1536,20 @@
       <c r="Q15" s="2">
         <v>21541.96</v>
       </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R15">
+        <v>22063.011016473039</v>
+      </c>
+      <c r="S15">
+        <v>-18383.886023922161</v>
+      </c>
+      <c r="T15">
+        <v>2.4017672602099012</v>
+      </c>
+      <c r="U15">
+        <v>1.1442300473160589</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>44409</v>
       </c>
@@ -1397,8 +1601,20 @@
       <c r="Q16" s="2">
         <v>21539.89</v>
       </c>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R16">
+        <v>22270.295068397369</v>
+      </c>
+      <c r="S16">
+        <v>-18354.980519791821</v>
+      </c>
+      <c r="T16">
+        <v>3.7694383456897009</v>
+      </c>
+      <c r="U16">
+        <v>0.95269023867037916</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>44440</v>
       </c>
@@ -1450,8 +1666,20 @@
       <c r="Q17" s="2">
         <v>21636.07</v>
       </c>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R17">
+        <v>22472.787669709629</v>
+      </c>
+      <c r="S17">
+        <v>-18414.520007901381</v>
+      </c>
+      <c r="T17">
+        <v>2.8306182630685042</v>
+      </c>
+      <c r="U17">
+        <v>1.07829177152692</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>44470</v>
       </c>
@@ -1503,8 +1731,20 @@
       <c r="Q18" s="2">
         <v>21900.48</v>
       </c>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R18">
+        <v>22678.822563455051</v>
+      </c>
+      <c r="S18">
+        <v>-18763.800376986339</v>
+      </c>
+      <c r="T18">
+        <v>2.9110190251035331</v>
+      </c>
+      <c r="U18">
+        <v>0.66834971397419451</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>44501</v>
       </c>
@@ -1556,8 +1796,20 @@
       <c r="Q19" s="2">
         <v>21905.88</v>
       </c>
-    </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R19">
+        <v>22914.15857083728</v>
+      </c>
+      <c r="S19">
+        <v>-18737.91035776474</v>
+      </c>
+      <c r="T19">
+        <v>3.558980588685682</v>
+      </c>
+      <c r="U19">
+        <v>1.2344199148499679</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>44531</v>
       </c>
@@ -1609,8 +1861,20 @@
       <c r="Q20" s="2">
         <v>22078.63</v>
       </c>
-    </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R20">
+        <v>23274.852756175522</v>
+      </c>
+      <c r="S20">
+        <v>-18845.228915190401</v>
+      </c>
+      <c r="T20">
+        <v>3.61753520699824</v>
+      </c>
+      <c r="U20">
+        <v>0.65541051549392781</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>44562</v>
       </c>
@@ -1662,8 +1926,20 @@
       <c r="Q21" s="2">
         <v>21890.75</v>
       </c>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R21">
+        <v>23252.81150330287</v>
+      </c>
+      <c r="S21">
+        <v>-18790.334340234622</v>
+      </c>
+      <c r="T21">
+        <v>3.311330397636628</v>
+      </c>
+      <c r="U21">
+        <v>0.93245549203178124</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>44593</v>
       </c>
@@ -1715,8 +1991,20 @@
       <c r="Q22" s="2">
         <v>21846.52</v>
       </c>
-    </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R22">
+        <v>23215.89147042382</v>
+      </c>
+      <c r="S22">
+        <v>-18755.6641150137</v>
+      </c>
+      <c r="T22">
+        <v>3.5409881209568121</v>
+      </c>
+      <c r="U22">
+        <v>0.713903236891966</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>44621</v>
       </c>
@@ -1768,8 +2056,20 @@
       <c r="Q23" s="2">
         <v>21978.03</v>
       </c>
-    </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R23">
+        <v>23495.214226148441</v>
+      </c>
+      <c r="S23">
+        <v>-18836.790281862352</v>
+      </c>
+      <c r="T23">
+        <v>3.3208454148431379</v>
+      </c>
+      <c r="U23">
+        <v>0.57085530133413664</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>44652</v>
       </c>
@@ -1821,8 +2121,20 @@
       <c r="Q24" s="2">
         <v>21945.02</v>
       </c>
-    </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R24">
+        <v>23587.533942972419</v>
+      </c>
+      <c r="S24">
+        <v>-18922.539102591571</v>
+      </c>
+      <c r="T24">
+        <v>3.988092967954167</v>
+      </c>
+      <c r="U24">
+        <v>0.78556320849638861</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>44682</v>
       </c>
@@ -1874,8 +2186,20 @@
       <c r="Q25" s="2">
         <v>21934.66</v>
       </c>
-    </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R25">
+        <v>23268.548735730728</v>
+      </c>
+      <c r="S25">
+        <v>-18954.993322130391</v>
+      </c>
+      <c r="T25">
+        <v>3.618621632824834</v>
+      </c>
+      <c r="U25">
+        <v>1.4149425217580329</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>44713</v>
       </c>
@@ -1927,8 +2251,20 @@
       <c r="Q26" s="2">
         <v>21881.66</v>
       </c>
-    </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R26">
+        <v>23251.705444071191</v>
+      </c>
+      <c r="S26">
+        <v>-18909.889934451239</v>
+      </c>
+      <c r="T26">
+        <v>2.497122845790912</v>
+      </c>
+      <c r="U26">
+        <v>0.65336229777322175</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>44743</v>
       </c>
@@ -1980,8 +2316,20 @@
       <c r="Q27" s="2">
         <v>21940.22</v>
       </c>
-    </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R27">
+        <v>23205.112166665709</v>
+      </c>
+      <c r="S27">
+        <v>-18940.604261408898</v>
+      </c>
+      <c r="T27">
+        <v>2.7456026166046388</v>
+      </c>
+      <c r="U27">
+        <v>0.7134602763039799</v>
+      </c>
+    </row>
+    <row r="28" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>44774</v>
       </c>
@@ -2033,8 +2381,20 @@
       <c r="Q28" s="2">
         <v>22182.86</v>
       </c>
-    </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R28">
+        <v>23153.90520596402</v>
+      </c>
+      <c r="S28">
+        <v>-19164.178065986689</v>
+      </c>
+      <c r="T28">
+        <v>3.6852333500854648</v>
+      </c>
+      <c r="U28">
+        <v>0.6072620725962512</v>
+      </c>
+    </row>
+    <row r="29" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>44805</v>
       </c>
@@ -2086,8 +2446,20 @@
       <c r="Q29" s="2">
         <v>22080.95</v>
       </c>
-    </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R29">
+        <v>22997.12437621611</v>
+      </c>
+      <c r="S29">
+        <v>-19093.570794072701</v>
+      </c>
+      <c r="T29">
+        <v>3.8492010908886169</v>
+      </c>
+      <c r="U29">
+        <v>1.0416240127568961</v>
+      </c>
+    </row>
+    <row r="30" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>44835</v>
       </c>
@@ -2139,8 +2511,20 @@
       <c r="Q30" s="2">
         <v>22227.78</v>
       </c>
-    </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R30">
+        <v>22809.018293312249</v>
+      </c>
+      <c r="S30">
+        <v>-19200.21058065999</v>
+      </c>
+      <c r="T30">
+        <v>3.7163125226284581</v>
+      </c>
+      <c r="U30">
+        <v>0.66671792401072949</v>
+      </c>
+    </row>
+    <row r="31" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>44866</v>
       </c>
@@ -2192,8 +2576,20 @@
       <c r="Q31" s="2">
         <v>22256.87</v>
       </c>
-    </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R31">
+        <v>22694.034350486021</v>
+      </c>
+      <c r="S31">
+        <v>-19241.229641830429</v>
+      </c>
+      <c r="T31">
+        <v>4.0744607899603071</v>
+      </c>
+      <c r="U31">
+        <v>1.992203679153091</v>
+      </c>
+    </row>
+    <row r="32" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>44896</v>
       </c>
@@ -2245,8 +2641,20 @@
       <c r="Q32" s="2">
         <v>22267.360000000001</v>
       </c>
-    </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R32">
+        <v>22623.206840527331</v>
+      </c>
+      <c r="S32">
+        <v>-19259.844704048912</v>
+      </c>
+      <c r="T32">
+        <v>2.4884858438580268</v>
+      </c>
+      <c r="U32">
+        <v>0.84549305695049026</v>
+      </c>
+    </row>
+    <row r="33" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>44927</v>
       </c>
@@ -2298,8 +2706,20 @@
       <c r="Q33" s="2">
         <v>22413.27</v>
       </c>
-    </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R33">
+        <v>22353.582034069659</v>
+      </c>
+      <c r="S33">
+        <v>-19421.547076127321</v>
+      </c>
+      <c r="T33">
+        <v>4.5950814895077956</v>
+      </c>
+      <c r="U33">
+        <v>1.497785720407887</v>
+      </c>
+    </row>
+    <row r="34" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
         <v>44958</v>
       </c>
@@ -2351,8 +2771,20 @@
       <c r="Q34" s="2">
         <v>22345.46</v>
       </c>
-    </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R34">
+        <v>22051.479638933899</v>
+      </c>
+      <c r="S34">
+        <v>-19400.41351143294</v>
+      </c>
+      <c r="T34">
+        <v>4.2724647206781876</v>
+      </c>
+      <c r="U34">
+        <v>0.91379915087974717</v>
+      </c>
+    </row>
+    <row r="35" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
         <v>44986</v>
       </c>
@@ -2404,8 +2836,20 @@
       <c r="Q35" s="2">
         <v>22455.21</v>
       </c>
-    </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R35">
+        <v>21852.78458165472</v>
+      </c>
+      <c r="S35">
+        <v>-19524.486399690741</v>
+      </c>
+      <c r="T35">
+        <v>4.5275626245576968</v>
+      </c>
+      <c r="U35">
+        <v>1.097500042427721</v>
+      </c>
+    </row>
+    <row r="36" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <v>45017</v>
       </c>
@@ -2457,8 +2901,20 @@
       <c r="Q36" s="2">
         <v>22451.62</v>
       </c>
-    </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R36">
+        <v>21554.807850852481</v>
+      </c>
+      <c r="S36">
+        <v>-19513.809233398079</v>
+      </c>
+      <c r="T36">
+        <v>3.5068546191123038</v>
+      </c>
+      <c r="U36">
+        <v>0.68547598864630199</v>
+      </c>
+    </row>
+    <row r="37" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
         <v>45047</v>
       </c>
@@ -2510,8 +2966,20 @@
       <c r="Q37" s="2">
         <v>22571.71</v>
       </c>
-    </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R37">
+        <v>21245.2192628177</v>
+      </c>
+      <c r="S37">
+        <v>-19661.60855040087</v>
+      </c>
+      <c r="T37">
+        <v>4.2873565925597266</v>
+      </c>
+      <c r="U37">
+        <v>1.5035600105238831</v>
+      </c>
+    </row>
+    <row r="38" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
         <v>45078</v>
       </c>
@@ -2563,8 +3031,20 @@
       <c r="Q38" s="2">
         <v>22598.78</v>
       </c>
-    </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R38">
+        <v>21202.258947418381</v>
+      </c>
+      <c r="S38">
+        <v>-19691.42941941338</v>
+      </c>
+      <c r="T38">
+        <v>5.165129218139394</v>
+      </c>
+      <c r="U38">
+        <v>0.90945122167107684</v>
+      </c>
+    </row>
+    <row r="39" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
         <v>45108</v>
       </c>
@@ -2616,8 +3096,20 @@
       <c r="Q39" s="2">
         <v>22691.1</v>
       </c>
-    </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R39">
+        <v>21117.593365559111</v>
+      </c>
+      <c r="S39">
+        <v>-19820.886902528899</v>
+      </c>
+      <c r="T39">
+        <v>4.0285159539751669</v>
+      </c>
+      <c r="U39">
+        <v>0.87878218176931155</v>
+      </c>
+    </row>
+    <row r="40" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
         <v>45139</v>
       </c>
@@ -2669,8 +3161,20 @@
       <c r="Q40" s="2">
         <v>22824.52</v>
       </c>
-    </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R40">
+        <v>21018.99657699572</v>
+      </c>
+      <c r="S40">
+        <v>-19953.050571865751</v>
+      </c>
+      <c r="T40">
+        <v>3.958391901123298</v>
+      </c>
+      <c r="U40">
+        <v>1.091249879391152</v>
+      </c>
+    </row>
+    <row r="41" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
         <v>45170</v>
       </c>
@@ -2722,8 +3226,20 @@
       <c r="Q41" s="2">
         <v>22831.06</v>
       </c>
-    </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R41">
+        <v>20936.899600270201</v>
+      </c>
+      <c r="S41">
+        <v>-19969.627273857652</v>
+      </c>
+      <c r="T41">
+        <v>4.5034866174139996</v>
+      </c>
+      <c r="U41">
+        <v>1.090301645252828</v>
+      </c>
+    </row>
+    <row r="42" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
         <v>45200</v>
       </c>
@@ -2775,8 +3291,20 @@
       <c r="Q42" s="2">
         <v>22791.99</v>
       </c>
-    </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R42">
+        <v>20823.488663932789</v>
+      </c>
+      <c r="S42">
+        <v>-19972.62796504483</v>
+      </c>
+      <c r="T42">
+        <v>6.1755973379301361</v>
+      </c>
+      <c r="U42">
+        <v>0.9826132565782717</v>
+      </c>
+    </row>
+    <row r="43" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
         <v>45231</v>
       </c>
@@ -2828,8 +3356,20 @@
       <c r="Q43" s="2">
         <v>22929.22</v>
       </c>
-    </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R43">
+        <v>20812.989407526329</v>
+      </c>
+      <c r="S43">
+        <v>-20096.660020525062</v>
+      </c>
+      <c r="T43">
+        <v>5.0033410676197114</v>
+      </c>
+      <c r="U43">
+        <v>1.253878361503048</v>
+      </c>
+    </row>
+    <row r="44" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
         <v>45261</v>
       </c>
@@ -2881,8 +3421,20 @@
       <c r="Q44" s="2">
         <v>23164.34</v>
       </c>
-    </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R44">
+        <v>20944.096402637198</v>
+      </c>
+      <c r="S44">
+        <v>-20289.683722559901</v>
+      </c>
+      <c r="T44">
+        <v>4.2993316701475646</v>
+      </c>
+      <c r="U44">
+        <v>1.2614540610906451</v>
+      </c>
+    </row>
+    <row r="45" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
         <v>45292</v>
       </c>
@@ -2934,8 +3486,20 @@
       <c r="Q45" s="2">
         <v>22958.54</v>
       </c>
-    </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R45">
+        <v>20837.2316150226</v>
+      </c>
+      <c r="S45">
+        <v>-20159.675408051069</v>
+      </c>
+      <c r="T45">
+        <v>4.3443776862552959</v>
+      </c>
+      <c r="U45">
+        <v>1.0147271323864819</v>
+      </c>
+    </row>
+    <row r="46" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
         <v>45323</v>
       </c>
@@ -2987,8 +3551,20 @@
       <c r="Q46" s="2">
         <v>23097.200000000001</v>
       </c>
-    </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R46">
+        <v>20755.723626830419</v>
+      </c>
+      <c r="S46">
+        <v>-20294.302953582312</v>
+      </c>
+      <c r="T46">
+        <v>4.0213433684774786</v>
+      </c>
+      <c r="U46">
+        <v>1.0196012324709911</v>
+      </c>
+    </row>
+    <row r="47" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
         <v>45352</v>
       </c>
@@ -3040,8 +3616,20 @@
       <c r="Q47" s="2">
         <v>23108.799999999999</v>
       </c>
-    </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R47">
+        <v>20931.017522296679</v>
+      </c>
+      <c r="S47">
+        <v>-20281.805526035201</v>
+      </c>
+      <c r="T47">
+        <v>4.5989061319682554</v>
+      </c>
+      <c r="U47">
+        <v>1.44738608879959</v>
+      </c>
+    </row>
+    <row r="48" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
         <v>45383</v>
       </c>
@@ -3093,8 +3681,20 @@
       <c r="Q48" s="2">
         <v>23164.39</v>
       </c>
-    </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R48">
+        <v>20974.84404596833</v>
+      </c>
+      <c r="S48">
+        <v>-20367.885670566051</v>
+      </c>
+      <c r="T48">
+        <v>2.861611830000363</v>
+      </c>
+      <c r="U48">
+        <v>1.233584490977234</v>
+      </c>
+    </row>
+    <row r="49" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
         <v>45413</v>
       </c>
@@ -3146,8 +3746,20 @@
       <c r="Q49" s="2">
         <v>23250.14</v>
       </c>
-    </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R49">
+        <v>20803.711308908569</v>
+      </c>
+      <c r="S49">
+        <v>-20466.89921579033</v>
+      </c>
+      <c r="T49">
+        <v>3.4784737906718028</v>
+      </c>
+      <c r="U49">
+        <v>1.0522160156146569</v>
+      </c>
+    </row>
+    <row r="50" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
         <v>45444</v>
       </c>
@@ -3199,8 +3811,20 @@
       <c r="Q50" s="2">
         <v>23261.08</v>
       </c>
-    </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R50">
+        <v>20901.99045711683</v>
+      </c>
+      <c r="S50">
+        <v>-20463.846307238509</v>
+      </c>
+      <c r="T50">
+        <v>4.3642795322534864</v>
+      </c>
+      <c r="U50">
+        <v>1.408944616056562</v>
+      </c>
+    </row>
+    <row r="51" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
         <v>45474</v>
       </c>
@@ -3252,8 +3876,20 @@
       <c r="Q51" s="2">
         <v>23400.78</v>
       </c>
-    </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R51">
+        <v>20900.491149350539</v>
+      </c>
+      <c r="S51">
+        <v>-20645.350208865941</v>
+      </c>
+      <c r="T51">
+        <v>5.0177202492208064</v>
+      </c>
+      <c r="U51">
+        <v>1.4839509653945691</v>
+      </c>
+    </row>
+    <row r="52" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
         <v>45505</v>
       </c>
@@ -3305,8 +3941,20 @@
       <c r="Q52" s="2">
         <v>23412.69</v>
       </c>
-    </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R52">
+        <v>20967.850410626361</v>
+      </c>
+      <c r="S52">
+        <v>-20647.204181620611</v>
+      </c>
+      <c r="T52">
+        <v>3.812181224166054</v>
+      </c>
+      <c r="U52">
+        <v>1.134805133582302</v>
+      </c>
+    </row>
+    <row r="53" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
         <v>45536</v>
       </c>
@@ -3358,8 +4006,20 @@
       <c r="Q53" s="2">
         <v>23391.4</v>
       </c>
-    </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R53">
+        <v>21033.703775814949</v>
+      </c>
+      <c r="S53">
+        <v>-20619.577516078651</v>
+      </c>
+      <c r="T53">
+        <v>3.5586088368397051</v>
+      </c>
+      <c r="U53">
+        <v>0.8428892082532472</v>
+      </c>
+    </row>
+    <row r="54" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A54" s="1">
         <v>45566</v>
       </c>
@@ -3411,8 +4071,20 @@
       <c r="Q54" s="2">
         <v>23528.19</v>
       </c>
-    </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R54">
+        <v>21084.004026736591</v>
+      </c>
+      <c r="S54">
+        <v>-20727.368974149729</v>
+      </c>
+      <c r="T54">
+        <v>4.4284741133921539</v>
+      </c>
+      <c r="U54">
+        <v>1.2987488945430219</v>
+      </c>
+    </row>
+    <row r="55" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A55" s="1">
         <v>45597</v>
       </c>
@@ -3464,8 +4136,20 @@
       <c r="Q55" s="2">
         <v>23587.96</v>
       </c>
-    </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R55">
+        <v>21263.883916715102</v>
+      </c>
+      <c r="S55">
+        <v>-20757.29425793824</v>
+      </c>
+      <c r="T55">
+        <v>4.3588683597750153</v>
+      </c>
+      <c r="U55">
+        <v>1.41556995626024</v>
+      </c>
+    </row>
+    <row r="56" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A56" s="1">
         <v>45627</v>
       </c>
@@ -3517,8 +4201,20 @@
       <c r="Q56" s="2">
         <v>23514.9</v>
       </c>
-    </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R56">
+        <v>21428.817933311209</v>
+      </c>
+      <c r="S56">
+        <v>-20670.448684940689</v>
+      </c>
+      <c r="T56">
+        <v>2.5664146248669288</v>
+      </c>
+      <c r="U56">
+        <v>0.9830613143721445</v>
+      </c>
+    </row>
+    <row r="57" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A57" s="1">
         <v>45658</v>
       </c>
@@ -3569,6 +4265,18 @@
       </c>
       <c r="Q57" s="2">
         <v>23552.74</v>
+      </c>
+      <c r="R57">
+        <v>21426.33148968609</v>
+      </c>
+      <c r="S57">
+        <v>-20867.082618338129</v>
+      </c>
+      <c r="T57">
+        <v>3.290558202446983</v>
+      </c>
+      <c r="U57">
+        <v>0.87296742189159271</v>
       </c>
     </row>
   </sheetData>

</xml_diff>